<commit_message>
fixed a C-code redundancy in template, added Customers Folder back to repo
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\code\PDF_host_Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2849311F-F412-48D3-A4C3-F6067A0F0067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A612030-8FD4-4E3F-B07E-3031755010DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7752" yWindow="696" windowWidth="13032" windowHeight="10032" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DavidSheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3525" uniqueCount="3253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3525" uniqueCount="3254">
   <si>
     <t>C-VI096</t>
   </si>
@@ -9779,16 +9779,25 @@
   </si>
   <si>
     <t>T-CI169</t>
+  </si>
+  <si>
+    <t>2722</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -10127,8 +10136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
+      <selection activeCell="C383" sqref="C383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13710,7 +13719,7 @@
         <v>849</v>
       </c>
       <c r="C379" t="s">
-        <v>592</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
@@ -23476,6 +23485,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed errors in template.xlsx, stringified poolID in GC2.py, reran and thus changed Customers Folder
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\code\PDF_host_Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A612030-8FD4-4E3F-B07E-3031755010DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0826E66-4301-49CC-B984-849DBDCECC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7752" yWindow="696" windowWidth="13032" windowHeight="10032" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DavidSheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3525" uniqueCount="3254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3524" uniqueCount="3254">
   <si>
     <t>C-VI096</t>
   </si>
@@ -10136,8 +10136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
-      <selection activeCell="C383" sqref="C383"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19313,8 +19313,8 @@
       <c r="A967" t="s">
         <v>2190</v>
       </c>
-      <c r="B967" t="s">
-        <v>2191</v>
+      <c r="B967">
+        <v>2785</v>
       </c>
     </row>
     <row r="968" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>